<commit_message>
Inventory Table created in Handlebars
</commit_message>
<xml_diff>
--- a/misc/relationalTableDraftThree.xlsx
+++ b/misc/relationalTableDraftThree.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah\Project2-Group2\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TONRIN\Project2-Group2\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3801FCD-F3F9-4003-B774-C5F23CBC502E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="109">
   <si>
     <t>ToyName</t>
   </si>
@@ -365,11 +366,14 @@
   <si>
     <t>Question5</t>
   </si>
+  <si>
+    <t>img</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -805,7 +809,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B6:Q20"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -1378,7 +1382,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:R27"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
@@ -2050,11 +2054,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A2:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,15 +2067,15 @@
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -2079,12 +2083,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -2092,12 +2096,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>87</v>
       </c>
@@ -2120,33 +2124,36 @@
         <v>61</v>
       </c>
       <c r="H11" t="s">
+        <v>108</v>
+      </c>
+      <c r="I11" t="s">
         <v>96</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>97</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>103</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>104</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>105</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>106</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>99</v>
       </c>

</xml_diff>